<commit_message>
tambah file csv pert1
</commit_message>
<xml_diff>
--- a/3SI1.xlsx
+++ b/3SI1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STIS\Semester 6\4.Analisis Peubah Ganda\R\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0437F7E-EAD4-49C2-9881-88E77179EE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDAB953-8D43-4922-ADF0-30827A523BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{DCE3E97D-BB80-46C9-AA7F-73A6A177A2E1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{DCE3E97D-BB80-46C9-AA7F-73A6A177A2E1}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -484,12 +484,12 @@
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="9.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.90625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -518,7 +518,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -547,7 +547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -576,7 +576,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -605,7 +605,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -634,7 +634,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -663,7 +663,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -692,7 +692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -721,7 +721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>8</v>
       </c>
@@ -750,7 +750,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>9</v>
       </c>
@@ -779,7 +779,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>10</v>
       </c>
@@ -808,7 +808,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>11</v>
       </c>
@@ -837,7 +837,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>12</v>
       </c>
@@ -866,7 +866,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>13</v>
       </c>
@@ -895,7 +895,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>14</v>
       </c>
@@ -924,7 +924,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>15</v>
       </c>
@@ -953,7 +953,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>16</v>
       </c>
@@ -982,7 +982,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1430,17 +1430,17 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>

</xml_diff>